<commit_message>
Updated files to include Vaccination
Added vaccination at the district and governorater levels. Updated the mat file for incidence. Wrote additional functions to compute the indirect impact of components.
</commit_message>
<xml_diff>
--- a/District and Cities info.xlsx
+++ b/District and Cities info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chadr\Desktop\Cholera-Methods\Cholera-Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72975B8-2597-4FC6-A719-58928154B27D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC63F06-B7AB-436E-AFFF-BF27122E777E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5730" yWindow="3975" windowWidth="21600" windowHeight="11400" xr2:uid="{7E40805A-7E38-4CB6-9B39-57193BD33F8A}"/>
+    <workbookView xWindow="-9165" yWindow="2190" windowWidth="21600" windowHeight="11400" xr2:uid="{7E40805A-7E38-4CB6-9B39-57193BD33F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Static_Info" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Al Hali</t>
   </si>
@@ -139,6 +139,18 @@
   <si>
     <t>Aden</t>
   </si>
+  <si>
+    <t xml:space="preserve"> FS PIN (2016)</t>
+  </si>
+  <si>
+    <t>FS PIN (2017)</t>
+  </si>
+  <si>
+    <t>FS PIN (2018)</t>
+  </si>
+  <si>
+    <t>FS PIN (2019)</t>
+  </si>
 </sst>
 </file>
 
@@ -147,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1009]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +201,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF454545"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -215,12 +233,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -234,7 +267,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -248,6 +281,10 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -568,7 +605,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,9 +614,11 @@
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -604,8 +643,20 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -634,8 +685,21 @@
       <c r="I2" s="2">
         <v>45701</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J2" s="3">
+        <f>K2*J$27/K$27</f>
+        <v>166250</v>
+      </c>
+      <c r="K2" s="13">
+        <v>70000</v>
+      </c>
+      <c r="L2">
+        <v>90252</v>
+      </c>
+      <c r="M2">
+        <v>49000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -664,8 +728,21 @@
       <c r="I3" s="2">
         <v>61710</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J22" si="0">K3*J$27/K$27</f>
+        <v>180500</v>
+      </c>
+      <c r="K3" s="13">
+        <v>76000</v>
+      </c>
+      <c r="L3">
+        <v>172151</v>
+      </c>
+      <c r="M3">
+        <v>69500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -694,8 +771,21 @@
       <c r="I4" s="2">
         <v>24848</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
+        <v>90250</v>
+      </c>
+      <c r="K4" s="13">
+        <v>38000</v>
+      </c>
+      <c r="L4">
+        <v>41323</v>
+      </c>
+      <c r="M4">
+        <v>28500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -712,7 +802,7 @@
         <v>200767</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F14" si="0">G5*F$28/G$28</f>
+        <f t="shared" ref="F5:F14" si="1">G5*F$28/G$28</f>
         <v>76517.356819080742</v>
       </c>
       <c r="G5" s="2">
@@ -724,8 +814,21 @@
       <c r="I5" s="2">
         <v>90345</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J5" s="3">
+        <f t="shared" si="0"/>
+        <v>68875</v>
+      </c>
+      <c r="K5" s="13">
+        <v>29000</v>
+      </c>
+      <c r="L5">
+        <v>131727</v>
+      </c>
+      <c r="M5">
+        <v>161000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -742,7 +845,7 @@
         <v>611867</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>337322.99555453903</v>
       </c>
       <c r="G6" s="2">
@@ -754,8 +857,21 @@
       <c r="I6" s="2">
         <v>367120</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="3">
+        <f t="shared" si="0"/>
+        <v>270750</v>
+      </c>
+      <c r="K6" s="13">
+        <v>114000</v>
+      </c>
+      <c r="L6">
+        <v>254706</v>
+      </c>
+      <c r="M6">
+        <v>367000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -772,7 +888,7 @@
         <v>211550</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100226.96034048604</v>
       </c>
       <c r="G7" s="2">
@@ -784,8 +900,21 @@
       <c r="I7" s="2">
         <v>126930</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J7" s="3">
+        <f t="shared" si="0"/>
+        <v>114000</v>
+      </c>
+      <c r="K7" s="13">
+        <v>48000</v>
+      </c>
+      <c r="L7">
+        <v>58477</v>
+      </c>
+      <c r="M7">
+        <v>116000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -802,7 +931,7 @@
         <v>132473</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51730.044046702467</v>
       </c>
       <c r="G8" s="2">
@@ -814,8 +943,21 @@
       <c r="I8" s="2">
         <v>59613</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8" s="3">
+        <f t="shared" si="0"/>
+        <v>47500</v>
+      </c>
+      <c r="K8" s="13">
+        <v>20000</v>
+      </c>
+      <c r="L8">
+        <v>47077</v>
+      </c>
+      <c r="M8">
+        <v>99000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -832,7 +974,7 @@
         <v>357419</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>135791.36562259399</v>
       </c>
       <c r="G9" s="2">
@@ -844,8 +986,21 @@
       <c r="I9" s="2">
         <v>160839</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J9" s="3">
+        <f t="shared" si="0"/>
+        <v>296875</v>
+      </c>
+      <c r="K9" s="13">
+        <v>125000</v>
+      </c>
+      <c r="L9">
+        <v>70619</v>
+      </c>
+      <c r="M9">
+        <v>214500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -862,7 +1017,7 @@
         <v>237636</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>113159.47135216165</v>
       </c>
       <c r="G10" s="2">
@@ -874,8 +1029,21 @@
       <c r="I10" s="2">
         <v>142582</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10" s="3">
+        <f t="shared" si="0"/>
+        <v>159125</v>
+      </c>
+      <c r="K10" s="13">
+        <v>67000</v>
+      </c>
+      <c r="L10">
+        <v>14209</v>
+      </c>
+      <c r="M10">
+        <v>142500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -892,7 +1060,7 @@
         <v>461298</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>196143.0836770802</v>
       </c>
       <c r="G11" s="2">
@@ -904,8 +1072,21 @@
       <c r="I11" s="2">
         <v>276779</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J11" s="3">
+        <f t="shared" si="0"/>
+        <v>942875</v>
+      </c>
+      <c r="K11" s="13">
+        <v>397000</v>
+      </c>
+      <c r="L11">
+        <v>290647</v>
+      </c>
+      <c r="M11">
+        <v>276500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -922,7 +1103,7 @@
         <v>612350</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>301758.59027243109</v>
       </c>
       <c r="G12" s="2">
@@ -934,8 +1115,21 @@
       <c r="I12" s="2">
         <v>367410</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
+        <v>230375</v>
+      </c>
+      <c r="K12" s="13">
+        <v>97000</v>
+      </c>
+      <c r="L12">
+        <v>273606</v>
+      </c>
+      <c r="M12">
+        <v>367000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -952,7 +1146,7 @@
         <v>123688</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49574.625544756535</v>
       </c>
       <c r="G13" s="2">
@@ -964,8 +1158,21 @@
       <c r="I13" s="2">
         <v>37106</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J13" s="3">
+        <f t="shared" si="0"/>
+        <v>99750</v>
+      </c>
+      <c r="K13" s="13">
+        <v>42000</v>
+      </c>
+      <c r="L13">
+        <v>49427</v>
+      </c>
+      <c r="M13">
+        <v>80500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -982,7 +1189,7 @@
         <v>457595</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>230629.77970821518</v>
       </c>
       <c r="G14" s="2">
@@ -994,8 +1201,21 @@
       <c r="I14" s="2">
         <v>137279</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>372875</v>
+      </c>
+      <c r="K14" s="13">
+        <v>157000</v>
+      </c>
+      <c r="L14">
+        <v>150389</v>
+      </c>
+      <c r="M14">
+        <v>274500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1024,16 +1244,21 @@
       <c r="I15" s="2">
         <v>58632</v>
       </c>
-      <c r="K15" s="2">
-        <f>AVERAGE(G15:I15)</f>
-        <v>67305.333333333328</v>
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
+        <v>180500</v>
+      </c>
+      <c r="K15" s="13">
+        <v>76000</v>
       </c>
       <c r="L15">
-        <f>AVERAGE(G15/B15,H15/D15,I15/E15)</f>
-        <v>0.55110153278341978</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>122556</v>
+      </c>
+      <c r="M15">
+        <v>97500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1275,7 @@
         <v>170905</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" ref="F16:F22" si="1">G16*F$29/G$29</f>
+        <f t="shared" ref="F16:F22" si="2">G16*F$29/G$29</f>
         <v>62610.837624135638</v>
       </c>
       <c r="G16" s="2">
@@ -1062,13 +1287,18 @@
       <c r="I16" s="2">
         <v>76907</v>
       </c>
-      <c r="K16" s="2">
-        <f t="shared" ref="K16:K22" si="2">AVERAGE(G16:I16)</f>
-        <v>72404.333333333328</v>
+      <c r="J16" s="3">
+        <f t="shared" si="0"/>
+        <v>111625</v>
+      </c>
+      <c r="K16" s="13">
+        <v>47000</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L16:L22" si="3">AVERAGE(G16/B16,H16/D16,I16/E16)</f>
-        <v>0.44944146149188358</v>
+        <v>129674</v>
+      </c>
+      <c r="M16">
+        <v>81500</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1088,7 +1318,7 @@
         <v>80680</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31772.663868964355</v>
       </c>
       <c r="G17" s="2">
@@ -1100,13 +1330,18 @@
       <c r="I17" s="2">
         <v>48408</v>
       </c>
-      <c r="K17" s="2">
-        <f t="shared" si="2"/>
-        <v>39208.333333333336</v>
+      <c r="J17" s="3">
+        <f t="shared" si="0"/>
+        <v>152000</v>
+      </c>
+      <c r="K17" s="13">
+        <v>64000</v>
       </c>
       <c r="L17">
-        <f t="shared" si="3"/>
-        <v>0.50073327304002413</v>
+        <v>45391</v>
+      </c>
+      <c r="M17">
+        <v>36000</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1126,7 +1361,7 @@
         <v>177151</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86907.580582755443</v>
       </c>
       <c r="G18" s="2">
@@ -1138,13 +1373,18 @@
       <c r="I18" s="2">
         <v>79718</v>
       </c>
-      <c r="K18" s="2">
-        <f t="shared" si="2"/>
-        <v>82812.666666666672</v>
+      <c r="J18" s="3">
+        <f t="shared" si="0"/>
+        <v>201875</v>
+      </c>
+      <c r="K18" s="13">
+        <v>85000</v>
       </c>
       <c r="L18">
-        <f t="shared" si="3"/>
-        <v>0.49929134761602745</v>
+        <v>165031</v>
+      </c>
+      <c r="M18">
+        <v>124000</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1164,7 +1404,7 @@
         <v>91444</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46724.505689653459</v>
       </c>
       <c r="G19" s="2">
@@ -1176,13 +1416,18 @@
       <c r="I19" s="2">
         <v>41150</v>
       </c>
-      <c r="K19" s="2">
-        <f t="shared" si="2"/>
-        <v>43668.333333333336</v>
+      <c r="J19" s="3">
+        <f t="shared" si="0"/>
+        <v>64125</v>
+      </c>
+      <c r="K19" s="13">
+        <v>27000</v>
       </c>
       <c r="L19">
-        <f t="shared" si="3"/>
-        <v>0.49804271196018074</v>
+        <v>39855</v>
+      </c>
+      <c r="M19">
+        <v>36500</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1202,7 +1447,7 @@
         <v>129552</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49527.976031032667</v>
       </c>
       <c r="G20" s="2">
@@ -1214,13 +1459,18 @@
       <c r="I20" s="2">
         <v>58298</v>
       </c>
-      <c r="K20" s="2">
-        <f t="shared" si="2"/>
-        <v>61781</v>
+      <c r="J20" s="3">
+        <f t="shared" si="0"/>
+        <v>147250</v>
+      </c>
+      <c r="K20" s="13">
+        <v>62000</v>
       </c>
       <c r="L20">
-        <f t="shared" si="3"/>
-        <v>0.50041778895990741</v>
+        <v>83918</v>
+      </c>
+      <c r="M20">
+        <v>71500</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1240,7 +1490,7 @@
         <v>144666</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70086.758534480192</v>
       </c>
       <c r="G21" s="2">
@@ -1252,13 +1502,18 @@
       <c r="I21" s="2">
         <v>86800</v>
       </c>
-      <c r="K21" s="2">
-        <f t="shared" si="2"/>
-        <v>81385</v>
+      <c r="J21" s="3">
+        <f t="shared" si="0"/>
+        <v>287375</v>
+      </c>
+      <c r="K21" s="13">
+        <v>121000</v>
       </c>
       <c r="L21">
-        <f t="shared" si="3"/>
-        <v>0.60116979335236176</v>
+        <v>133141</v>
+      </c>
+      <c r="M21">
+        <v>108500</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1278,7 +1533,7 @@
         <v>72617</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28034.703413792078</v>
       </c>
       <c r="G22" s="2">
@@ -1290,37 +1545,42 @@
       <c r="I22" s="2">
         <v>32678</v>
       </c>
-      <c r="K22" s="2">
-        <f t="shared" si="2"/>
-        <v>35403.333333333336</v>
+      <c r="J22" s="3">
+        <f t="shared" si="0"/>
+        <v>78375</v>
+      </c>
+      <c r="K22" s="13">
+        <v>33000</v>
       </c>
       <c r="L22">
-        <f t="shared" si="3"/>
-        <v>0.49990059478405052</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>44257</v>
+      </c>
+      <c r="M22">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" ref="B23:I23" si="4">SUM(B2:B4)</f>
+        <f t="shared" ref="B23:M23" si="3">SUM(B2:B4)</f>
         <v>577990</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>604544</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>606735</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>176344</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>282159.78773867548</v>
       </c>
       <c r="G23" s="2">
@@ -1328,15 +1588,31 @@
         <v>329000</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>364042</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>132259</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J23" s="2">
+        <f t="shared" si="3"/>
+        <v>437000</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="3"/>
+        <v>184000</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="3"/>
+        <v>303726</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="3"/>
+        <v>147000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1364,8 +1640,20 @@
       <c r="I24" s="2">
         <v>1766003</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J24" s="14">
+        <v>3094000</v>
+      </c>
+      <c r="K24" s="14">
+        <v>1096000</v>
+      </c>
+      <c r="L24" s="14">
+        <v>1340884</v>
+      </c>
+      <c r="M24" s="14">
+        <v>2098500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1393,8 +1681,21 @@
       <c r="I25">
         <v>482591</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J25" s="14">
+        <v>895000</v>
+      </c>
+      <c r="K25" s="14">
+        <v>515000</v>
+      </c>
+      <c r="L25" s="14">
+        <v>763823</v>
+      </c>
+      <c r="M25" s="14">
+        <v>588500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1422,12 +1723,23 @@
       <c r="I27">
         <v>2087080</v>
       </c>
-      <c r="M27" s="2"/>
+      <c r="J27" s="14">
+        <v>3097000</v>
+      </c>
+      <c r="K27" s="14">
+        <v>1304000</v>
+      </c>
+      <c r="L27" s="14">
+        <v>1960171</v>
+      </c>
+      <c r="M27" s="14">
+        <v>2048000</v>
+      </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1455,12 +1767,23 @@
       <c r="I28" s="2">
         <v>1766003</v>
       </c>
-      <c r="M28" s="2"/>
+      <c r="J28" s="14">
+        <v>3094000</v>
+      </c>
+      <c r="K28" s="14">
+        <v>1096000</v>
+      </c>
+      <c r="L28" s="14">
+        <v>1340884</v>
+      </c>
+      <c r="M28" s="14">
+        <v>2098500</v>
+      </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1487,6 +1810,18 @@
       </c>
       <c r="I29">
         <v>482591</v>
+      </c>
+      <c r="J29" s="14">
+        <v>895000</v>
+      </c>
+      <c r="K29" s="14">
+        <v>515000</v>
+      </c>
+      <c r="L29" s="14">
+        <v>763823</v>
+      </c>
+      <c r="M29" s="14">
+        <v>588500</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -1508,280 +1843,126 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="2">
-        <v>114370</v>
-      </c>
-      <c r="E33" s="2">
-        <v>69000</v>
-      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="2">
-        <v>149446</v>
-      </c>
-      <c r="E34" s="2">
-        <v>67000</v>
-      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="2">
-        <v>75188</v>
-      </c>
-      <c r="E35" s="2">
-        <v>34000</v>
-      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="2">
-        <v>155551</v>
-      </c>
-      <c r="E36" s="2">
-        <v>93000</v>
-      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="2">
-        <v>84157</v>
-      </c>
-      <c r="E37" s="2">
-        <v>50000</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K37" s="2">
-        <v>71000</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N37" s="2">
-        <v>158523</v>
-      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="2">
-        <v>117449</v>
-      </c>
-      <c r="E38" s="2">
-        <v>53000</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" s="2">
-        <v>313000</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N38" s="2">
-        <v>522488</v>
-      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" s="2">
-        <v>124274</v>
-      </c>
-      <c r="E39" s="2">
-        <v>75000</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K39" s="2">
-        <v>93000</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N39" s="2">
-        <v>155460</v>
-      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="2">
-        <v>66712</v>
-      </c>
-      <c r="E40" s="2">
-        <v>30000</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K40" s="2">
-        <v>48000</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N40" s="2">
-        <v>106145</v>
-      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="J41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K41" s="2">
-        <v>126000</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N41" s="2">
-        <v>280532</v>
-      </c>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="J42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K42" s="2">
-        <v>105000</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N42" s="2">
-        <v>175059</v>
-      </c>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="2">
-        <v>239552</v>
-      </c>
-      <c r="E43" s="2">
-        <v>144000</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K43" s="2">
-        <v>182000</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N43" s="2">
-        <v>303930</v>
-      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="2">
-        <v>217122</v>
-      </c>
-      <c r="E44" s="2">
-        <v>130000</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K44" s="2">
-        <v>280000</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N44" s="2">
-        <v>466113</v>
-      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="2">
-        <v>121316</v>
-      </c>
-      <c r="E45" s="2">
-        <v>55000</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K45" s="2">
-        <v>46000</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N45" s="2">
-        <v>103316</v>
-      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="J46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K46" s="2">
-        <v>214000</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N46" s="2">
-        <v>356472</v>
-      </c>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B43:E45">

</xml_diff>